<commit_message>
Jenkins plug-in and other corrections
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/resource/ScenarioStatus.xlsx
+++ b/src/test/java/ApachePOI/resource/ScenarioStatus.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="16">
   <si>
     <t>Create a country</t>
   </si>
@@ -58,6 +58,9 @@
   <si>
     <t>13.10.22</t>
   </si>
+  <si>
+    <t>02.11.22</t>
+  </si>
 </sst>
 </file>
 
@@ -101,7 +104,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D159"/>
+  <dimension ref="A1:D211"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -2333,6 +2336,734 @@
         <v>14</v>
       </c>
     </row>
+    <row r="160">
+      <c r="A160" t="s">
+        <v>9</v>
+      </c>
+      <c r="B160" t="s">
+        <v>1</v>
+      </c>
+      <c r="C160" t="s">
+        <v>2</v>
+      </c>
+      <c r="D160" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="s">
+        <v>9</v>
+      </c>
+      <c r="B161" t="s">
+        <v>1</v>
+      </c>
+      <c r="C161" t="s">
+        <v>2</v>
+      </c>
+      <c r="D161" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="s">
+        <v>9</v>
+      </c>
+      <c r="B162" t="s">
+        <v>1</v>
+      </c>
+      <c r="C162" t="s">
+        <v>2</v>
+      </c>
+      <c r="D162" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="s">
+        <v>9</v>
+      </c>
+      <c r="B163" t="s">
+        <v>1</v>
+      </c>
+      <c r="C163" t="s">
+        <v>2</v>
+      </c>
+      <c r="D163" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="s">
+        <v>9</v>
+      </c>
+      <c r="B164" t="s">
+        <v>1</v>
+      </c>
+      <c r="C164" t="s">
+        <v>2</v>
+      </c>
+      <c r="D164" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="s">
+        <v>9</v>
+      </c>
+      <c r="B165" t="s">
+        <v>1</v>
+      </c>
+      <c r="C165" t="s">
+        <v>2</v>
+      </c>
+      <c r="D165" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="s">
+        <v>9</v>
+      </c>
+      <c r="B166" t="s">
+        <v>1</v>
+      </c>
+      <c r="C166" t="s">
+        <v>2</v>
+      </c>
+      <c r="D166" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="s">
+        <v>9</v>
+      </c>
+      <c r="B167" t="s">
+        <v>1</v>
+      </c>
+      <c r="C167" t="s">
+        <v>2</v>
+      </c>
+      <c r="D167" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="s">
+        <v>9</v>
+      </c>
+      <c r="B168" t="s">
+        <v>1</v>
+      </c>
+      <c r="C168" t="s">
+        <v>2</v>
+      </c>
+      <c r="D168" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="s">
+        <v>7</v>
+      </c>
+      <c r="B169" t="s">
+        <v>1</v>
+      </c>
+      <c r="C169" t="s">
+        <v>2</v>
+      </c>
+      <c r="D169" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="s">
+        <v>9</v>
+      </c>
+      <c r="B170" t="s">
+        <v>1</v>
+      </c>
+      <c r="C170" t="s">
+        <v>2</v>
+      </c>
+      <c r="D170" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="s">
+        <v>9</v>
+      </c>
+      <c r="B171" t="s">
+        <v>1</v>
+      </c>
+      <c r="C171" t="s">
+        <v>2</v>
+      </c>
+      <c r="D171" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="s">
+        <v>9</v>
+      </c>
+      <c r="B172" t="s">
+        <v>1</v>
+      </c>
+      <c r="C172" t="s">
+        <v>2</v>
+      </c>
+      <c r="D172" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="s">
+        <v>9</v>
+      </c>
+      <c r="B173" t="s">
+        <v>1</v>
+      </c>
+      <c r="C173" t="s">
+        <v>2</v>
+      </c>
+      <c r="D173" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="s">
+        <v>9</v>
+      </c>
+      <c r="B174" t="s">
+        <v>1</v>
+      </c>
+      <c r="C174" t="s">
+        <v>2</v>
+      </c>
+      <c r="D174" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="s">
+        <v>9</v>
+      </c>
+      <c r="B175" t="s">
+        <v>1</v>
+      </c>
+      <c r="C175" t="s">
+        <v>2</v>
+      </c>
+      <c r="D175" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="s">
+        <v>9</v>
+      </c>
+      <c r="B176" t="s">
+        <v>6</v>
+      </c>
+      <c r="C176" t="s">
+        <v>2</v>
+      </c>
+      <c r="D176" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="s">
+        <v>9</v>
+      </c>
+      <c r="B177" t="s">
+        <v>6</v>
+      </c>
+      <c r="C177" t="s">
+        <v>2</v>
+      </c>
+      <c r="D177" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="s">
+        <v>9</v>
+      </c>
+      <c r="B178" t="s">
+        <v>1</v>
+      </c>
+      <c r="C178" t="s">
+        <v>4</v>
+      </c>
+      <c r="D178" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="s">
+        <v>9</v>
+      </c>
+      <c r="B179" t="s">
+        <v>1</v>
+      </c>
+      <c r="C179" t="s">
+        <v>2</v>
+      </c>
+      <c r="D179" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="s">
+        <v>9</v>
+      </c>
+      <c r="B180" t="s">
+        <v>6</v>
+      </c>
+      <c r="C180" t="s">
+        <v>4</v>
+      </c>
+      <c r="D180" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="s">
+        <v>9</v>
+      </c>
+      <c r="B181" t="s">
+        <v>1</v>
+      </c>
+      <c r="C181" t="s">
+        <v>2</v>
+      </c>
+      <c r="D181" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="s">
+        <v>9</v>
+      </c>
+      <c r="B182" t="s">
+        <v>1</v>
+      </c>
+      <c r="C182" t="s">
+        <v>4</v>
+      </c>
+      <c r="D182" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="s">
+        <v>9</v>
+      </c>
+      <c r="B183" t="s">
+        <v>1</v>
+      </c>
+      <c r="C183" t="s">
+        <v>2</v>
+      </c>
+      <c r="D183" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="s">
+        <v>9</v>
+      </c>
+      <c r="B184" t="s">
+        <v>1</v>
+      </c>
+      <c r="C184" t="s">
+        <v>4</v>
+      </c>
+      <c r="D184" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="s">
+        <v>9</v>
+      </c>
+      <c r="B185" t="s">
+        <v>6</v>
+      </c>
+      <c r="C185" t="s">
+        <v>2</v>
+      </c>
+      <c r="D185" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="s">
+        <v>9</v>
+      </c>
+      <c r="B186" t="s">
+        <v>6</v>
+      </c>
+      <c r="C186" t="s">
+        <v>4</v>
+      </c>
+      <c r="D186" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="s">
+        <v>9</v>
+      </c>
+      <c r="B187" t="s">
+        <v>6</v>
+      </c>
+      <c r="C187" t="s">
+        <v>4</v>
+      </c>
+      <c r="D187" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="s">
+        <v>9</v>
+      </c>
+      <c r="B188" t="s">
+        <v>1</v>
+      </c>
+      <c r="C188" t="s">
+        <v>2</v>
+      </c>
+      <c r="D188" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="s">
+        <v>9</v>
+      </c>
+      <c r="B189" t="s">
+        <v>1</v>
+      </c>
+      <c r="C189" t="s">
+        <v>4</v>
+      </c>
+      <c r="D189" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="s">
+        <v>9</v>
+      </c>
+      <c r="B190" t="s">
+        <v>6</v>
+      </c>
+      <c r="C190" t="s">
+        <v>2</v>
+      </c>
+      <c r="D190" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="s">
+        <v>9</v>
+      </c>
+      <c r="B191" t="s">
+        <v>1</v>
+      </c>
+      <c r="C191" t="s">
+        <v>4</v>
+      </c>
+      <c r="D191" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="s">
+        <v>9</v>
+      </c>
+      <c r="B192" t="s">
+        <v>6</v>
+      </c>
+      <c r="C192" t="s">
+        <v>2</v>
+      </c>
+      <c r="D192" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="s">
+        <v>9</v>
+      </c>
+      <c r="B193" t="s">
+        <v>1</v>
+      </c>
+      <c r="C193" t="s">
+        <v>4</v>
+      </c>
+      <c r="D193" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="s">
+        <v>9</v>
+      </c>
+      <c r="B194" t="s">
+        <v>1</v>
+      </c>
+      <c r="C194" t="s">
+        <v>2</v>
+      </c>
+      <c r="D194" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="s">
+        <v>9</v>
+      </c>
+      <c r="B195" t="s">
+        <v>6</v>
+      </c>
+      <c r="C195" t="s">
+        <v>2</v>
+      </c>
+      <c r="D195" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="s">
+        <v>9</v>
+      </c>
+      <c r="B196" t="s">
+        <v>6</v>
+      </c>
+      <c r="C196" t="s">
+        <v>4</v>
+      </c>
+      <c r="D196" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="s">
+        <v>7</v>
+      </c>
+      <c r="B197" t="s">
+        <v>1</v>
+      </c>
+      <c r="C197" t="s">
+        <v>2</v>
+      </c>
+      <c r="D197" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="s">
+        <v>9</v>
+      </c>
+      <c r="B198" t="s">
+        <v>1</v>
+      </c>
+      <c r="C198" t="s">
+        <v>2</v>
+      </c>
+      <c r="D198" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="s">
+        <v>9</v>
+      </c>
+      <c r="B199" t="s">
+        <v>1</v>
+      </c>
+      <c r="C199" t="s">
+        <v>2</v>
+      </c>
+      <c r="D199" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="s">
+        <v>9</v>
+      </c>
+      <c r="B200" t="s">
+        <v>1</v>
+      </c>
+      <c r="C200" t="s">
+        <v>2</v>
+      </c>
+      <c r="D200" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="s">
+        <v>9</v>
+      </c>
+      <c r="B201" t="s">
+        <v>1</v>
+      </c>
+      <c r="C201" t="s">
+        <v>2</v>
+      </c>
+      <c r="D201" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="s">
+        <v>9</v>
+      </c>
+      <c r="B202" t="s">
+        <v>1</v>
+      </c>
+      <c r="C202" t="s">
+        <v>2</v>
+      </c>
+      <c r="D202" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="s">
+        <v>9</v>
+      </c>
+      <c r="B203" t="s">
+        <v>1</v>
+      </c>
+      <c r="C203" t="s">
+        <v>2</v>
+      </c>
+      <c r="D203" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="s">
+        <v>9</v>
+      </c>
+      <c r="B204" t="s">
+        <v>1</v>
+      </c>
+      <c r="C204" t="s">
+        <v>2</v>
+      </c>
+      <c r="D204" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="s">
+        <v>9</v>
+      </c>
+      <c r="B205" t="s">
+        <v>1</v>
+      </c>
+      <c r="C205" t="s">
+        <v>2</v>
+      </c>
+      <c r="D205" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="s">
+        <v>9</v>
+      </c>
+      <c r="B206" t="s">
+        <v>6</v>
+      </c>
+      <c r="C206" t="s">
+        <v>2</v>
+      </c>
+      <c r="D206" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="s">
+        <v>9</v>
+      </c>
+      <c r="B207" t="s">
+        <v>6</v>
+      </c>
+      <c r="C207" t="s">
+        <v>2</v>
+      </c>
+      <c r="D207" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="s">
+        <v>9</v>
+      </c>
+      <c r="B208" t="s">
+        <v>1</v>
+      </c>
+      <c r="C208" t="s">
+        <v>2</v>
+      </c>
+      <c r="D208" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="s">
+        <v>9</v>
+      </c>
+      <c r="B209" t="s">
+        <v>1</v>
+      </c>
+      <c r="C209" t="s">
+        <v>2</v>
+      </c>
+      <c r="D209" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="s">
+        <v>9</v>
+      </c>
+      <c r="B210" t="s">
+        <v>6</v>
+      </c>
+      <c r="C210" t="s">
+        <v>4</v>
+      </c>
+      <c r="D210" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="s">
+        <v>9</v>
+      </c>
+      <c r="B211" t="s">
+        <v>6</v>
+      </c>
+      <c r="C211" t="s">
+        <v>4</v>
+      </c>
+      <c r="D211" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Listeners class added to Runners.
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/resource/ScenarioStatus.xlsx
+++ b/src/test/java/ApachePOI/resource/ScenarioStatus.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="19">
   <si>
     <t>Create a country</t>
   </si>
@@ -113,7 +113,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D242"/>
+  <dimension ref="A1:D249"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -3507,6 +3507,104 @@
         <v>18</v>
       </c>
     </row>
+    <row r="243">
+      <c r="A243" t="s">
+        <v>7</v>
+      </c>
+      <c r="B243" t="s">
+        <v>1</v>
+      </c>
+      <c r="C243" t="s">
+        <v>2</v>
+      </c>
+      <c r="D243" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="s">
+        <v>9</v>
+      </c>
+      <c r="B244" t="s">
+        <v>6</v>
+      </c>
+      <c r="C244" t="s">
+        <v>2</v>
+      </c>
+      <c r="D244" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="s">
+        <v>9</v>
+      </c>
+      <c r="B245" t="s">
+        <v>6</v>
+      </c>
+      <c r="C245" t="s">
+        <v>2</v>
+      </c>
+      <c r="D245" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="s">
+        <v>9</v>
+      </c>
+      <c r="B246" t="s">
+        <v>6</v>
+      </c>
+      <c r="C246" t="s">
+        <v>2</v>
+      </c>
+      <c r="D246" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="s">
+        <v>9</v>
+      </c>
+      <c r="B247" t="s">
+        <v>1</v>
+      </c>
+      <c r="C247" t="s">
+        <v>2</v>
+      </c>
+      <c r="D247" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="s">
+        <v>9</v>
+      </c>
+      <c r="B248" t="s">
+        <v>1</v>
+      </c>
+      <c r="C248" t="s">
+        <v>2</v>
+      </c>
+      <c r="D248" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="s">
+        <v>9</v>
+      </c>
+      <c r="B249" t="s">
+        <v>1</v>
+      </c>
+      <c r="C249" t="s">
+        <v>2</v>
+      </c>
+      <c r="D249" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
url and credentials changed
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/resource/ScenarioStatus.xlsx
+++ b/src/test/java/ApachePOI/resource/ScenarioStatus.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1156" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="21">
   <si>
     <t>Create a country</t>
   </si>
@@ -73,6 +73,9 @@
   <si>
     <t>Login with one invalid pair of (username and password)</t>
   </si>
+  <si>
+    <t>29.12.22</t>
+  </si>
 </sst>
 </file>
 
@@ -116,7 +119,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D289"/>
+  <dimension ref="A1:D358"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -4168,6 +4171,972 @@
         <v>18</v>
       </c>
     </row>
+    <row r="290">
+      <c r="A290" t="s">
+        <v>9</v>
+      </c>
+      <c r="B290" t="s">
+        <v>6</v>
+      </c>
+      <c r="C290" t="s">
+        <v>13</v>
+      </c>
+      <c r="D290" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="s">
+        <v>9</v>
+      </c>
+      <c r="B291" t="s">
+        <v>6</v>
+      </c>
+      <c r="C291" t="s">
+        <v>13</v>
+      </c>
+      <c r="D291" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="s">
+        <v>9</v>
+      </c>
+      <c r="B292" t="s">
+        <v>6</v>
+      </c>
+      <c r="C292" t="s">
+        <v>13</v>
+      </c>
+      <c r="D292" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="s">
+        <v>9</v>
+      </c>
+      <c r="B293" t="s">
+        <v>6</v>
+      </c>
+      <c r="C293" t="s">
+        <v>4</v>
+      </c>
+      <c r="D293" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="s">
+        <v>9</v>
+      </c>
+      <c r="B294" t="s">
+        <v>6</v>
+      </c>
+      <c r="C294" t="s">
+        <v>4</v>
+      </c>
+      <c r="D294" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="s">
+        <v>9</v>
+      </c>
+      <c r="B295" t="s">
+        <v>6</v>
+      </c>
+      <c r="C295" t="s">
+        <v>4</v>
+      </c>
+      <c r="D295" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="s">
+        <v>9</v>
+      </c>
+      <c r="B296" t="s">
+        <v>6</v>
+      </c>
+      <c r="C296" t="s">
+        <v>13</v>
+      </c>
+      <c r="D296" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="s">
+        <v>9</v>
+      </c>
+      <c r="B297" t="s">
+        <v>1</v>
+      </c>
+      <c r="C297" t="s">
+        <v>2</v>
+      </c>
+      <c r="D297" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="s">
+        <v>9</v>
+      </c>
+      <c r="B298" t="s">
+        <v>6</v>
+      </c>
+      <c r="C298" t="s">
+        <v>13</v>
+      </c>
+      <c r="D298" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="s">
+        <v>9</v>
+      </c>
+      <c r="B299" t="s">
+        <v>6</v>
+      </c>
+      <c r="C299" t="s">
+        <v>13</v>
+      </c>
+      <c r="D299" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="s">
+        <v>9</v>
+      </c>
+      <c r="B300" t="s">
+        <v>6</v>
+      </c>
+      <c r="C300" t="s">
+        <v>2</v>
+      </c>
+      <c r="D300" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="s">
+        <v>9</v>
+      </c>
+      <c r="B301" t="s">
+        <v>1</v>
+      </c>
+      <c r="C301" t="s">
+        <v>2</v>
+      </c>
+      <c r="D301" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="s">
+        <v>9</v>
+      </c>
+      <c r="B302" t="s">
+        <v>6</v>
+      </c>
+      <c r="C302" t="s">
+        <v>13</v>
+      </c>
+      <c r="D302" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="s">
+        <v>9</v>
+      </c>
+      <c r="B303" t="s">
+        <v>6</v>
+      </c>
+      <c r="C303" t="s">
+        <v>13</v>
+      </c>
+      <c r="D303" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="s">
+        <v>9</v>
+      </c>
+      <c r="B304" t="s">
+        <v>6</v>
+      </c>
+      <c r="C304" t="s">
+        <v>13</v>
+      </c>
+      <c r="D304" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="s">
+        <v>9</v>
+      </c>
+      <c r="B305" t="s">
+        <v>1</v>
+      </c>
+      <c r="C305" t="s">
+        <v>2</v>
+      </c>
+      <c r="D305" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="s">
+        <v>9</v>
+      </c>
+      <c r="B306" t="s">
+        <v>6</v>
+      </c>
+      <c r="C306" t="s">
+        <v>13</v>
+      </c>
+      <c r="D306" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="s">
+        <v>9</v>
+      </c>
+      <c r="B307" t="s">
+        <v>1</v>
+      </c>
+      <c r="C307" t="s">
+        <v>2</v>
+      </c>
+      <c r="D307" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="s">
+        <v>9</v>
+      </c>
+      <c r="B308" t="s">
+        <v>1</v>
+      </c>
+      <c r="C308" t="s">
+        <v>2</v>
+      </c>
+      <c r="D308" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="s">
+        <v>9</v>
+      </c>
+      <c r="B309" t="s">
+        <v>6</v>
+      </c>
+      <c r="C309" t="s">
+        <v>13</v>
+      </c>
+      <c r="D309" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="s">
+        <v>9</v>
+      </c>
+      <c r="B310" t="s">
+        <v>1</v>
+      </c>
+      <c r="C310" t="s">
+        <v>2</v>
+      </c>
+      <c r="D310" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="s">
+        <v>9</v>
+      </c>
+      <c r="B311" t="s">
+        <v>1</v>
+      </c>
+      <c r="C311" t="s">
+        <v>4</v>
+      </c>
+      <c r="D311" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="s">
+        <v>9</v>
+      </c>
+      <c r="B312" t="s">
+        <v>1</v>
+      </c>
+      <c r="C312" t="s">
+        <v>2</v>
+      </c>
+      <c r="D312" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="s">
+        <v>9</v>
+      </c>
+      <c r="B313" t="s">
+        <v>6</v>
+      </c>
+      <c r="C313" t="s">
+        <v>4</v>
+      </c>
+      <c r="D313" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="s">
+        <v>9</v>
+      </c>
+      <c r="B314" t="s">
+        <v>1</v>
+      </c>
+      <c r="C314" t="s">
+        <v>2</v>
+      </c>
+      <c r="D314" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="s">
+        <v>7</v>
+      </c>
+      <c r="B315" t="s">
+        <v>6</v>
+      </c>
+      <c r="C315" t="s">
+        <v>2</v>
+      </c>
+      <c r="D315" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="s">
+        <v>19</v>
+      </c>
+      <c r="B316" t="s">
+        <v>6</v>
+      </c>
+      <c r="C316" t="s">
+        <v>2</v>
+      </c>
+      <c r="D316" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="s">
+        <v>19</v>
+      </c>
+      <c r="B317" t="s">
+        <v>6</v>
+      </c>
+      <c r="C317" t="s">
+        <v>2</v>
+      </c>
+      <c r="D317" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="s">
+        <v>19</v>
+      </c>
+      <c r="B318" t="s">
+        <v>6</v>
+      </c>
+      <c r="C318" t="s">
+        <v>2</v>
+      </c>
+      <c r="D318" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="s">
+        <v>7</v>
+      </c>
+      <c r="B319" t="s">
+        <v>1</v>
+      </c>
+      <c r="C319" t="s">
+        <v>2</v>
+      </c>
+      <c r="D319" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="s">
+        <v>19</v>
+      </c>
+      <c r="B320" t="s">
+        <v>1</v>
+      </c>
+      <c r="C320" t="s">
+        <v>2</v>
+      </c>
+      <c r="D320" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="s">
+        <v>19</v>
+      </c>
+      <c r="B321" t="s">
+        <v>1</v>
+      </c>
+      <c r="C321" t="s">
+        <v>2</v>
+      </c>
+      <c r="D321" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="s">
+        <v>19</v>
+      </c>
+      <c r="B322" t="s">
+        <v>1</v>
+      </c>
+      <c r="C322" t="s">
+        <v>2</v>
+      </c>
+      <c r="D322" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="s">
+        <v>9</v>
+      </c>
+      <c r="B323" t="s">
+        <v>1</v>
+      </c>
+      <c r="C323" t="s">
+        <v>2</v>
+      </c>
+      <c r="D323" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="s">
+        <v>9</v>
+      </c>
+      <c r="B324" t="s">
+        <v>1</v>
+      </c>
+      <c r="C324" t="s">
+        <v>2</v>
+      </c>
+      <c r="D324" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="s">
+        <v>9</v>
+      </c>
+      <c r="B325" t="s">
+        <v>1</v>
+      </c>
+      <c r="C325" t="s">
+        <v>2</v>
+      </c>
+      <c r="D325" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="s">
+        <v>9</v>
+      </c>
+      <c r="B326" t="s">
+        <v>1</v>
+      </c>
+      <c r="C326" t="s">
+        <v>2</v>
+      </c>
+      <c r="D326" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="s">
+        <v>9</v>
+      </c>
+      <c r="B327" t="s">
+        <v>6</v>
+      </c>
+      <c r="C327" t="s">
+        <v>4</v>
+      </c>
+      <c r="D327" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="s">
+        <v>9</v>
+      </c>
+      <c r="B328" t="s">
+        <v>1</v>
+      </c>
+      <c r="C328" t="s">
+        <v>2</v>
+      </c>
+      <c r="D328" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="s">
+        <v>9</v>
+      </c>
+      <c r="B329" t="s">
+        <v>6</v>
+      </c>
+      <c r="C329" t="s">
+        <v>4</v>
+      </c>
+      <c r="D329" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="s">
+        <v>9</v>
+      </c>
+      <c r="B330" t="s">
+        <v>1</v>
+      </c>
+      <c r="C330" t="s">
+        <v>2</v>
+      </c>
+      <c r="D330" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="s">
+        <v>9</v>
+      </c>
+      <c r="B331" t="s">
+        <v>1</v>
+      </c>
+      <c r="C331" t="s">
+        <v>2</v>
+      </c>
+      <c r="D331" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="s">
+        <v>9</v>
+      </c>
+      <c r="B332" t="s">
+        <v>1</v>
+      </c>
+      <c r="C332" t="s">
+        <v>4</v>
+      </c>
+      <c r="D332" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="s">
+        <v>9</v>
+      </c>
+      <c r="B333" t="s">
+        <v>1</v>
+      </c>
+      <c r="C333" t="s">
+        <v>2</v>
+      </c>
+      <c r="D333" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="s">
+        <v>9</v>
+      </c>
+      <c r="B334" t="s">
+        <v>6</v>
+      </c>
+      <c r="C334" t="s">
+        <v>4</v>
+      </c>
+      <c r="D334" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="s">
+        <v>9</v>
+      </c>
+      <c r="B335" t="s">
+        <v>6</v>
+      </c>
+      <c r="C335" t="s">
+        <v>4</v>
+      </c>
+      <c r="D335" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="s">
+        <v>9</v>
+      </c>
+      <c r="B336" t="s">
+        <v>1</v>
+      </c>
+      <c r="C336" t="s">
+        <v>2</v>
+      </c>
+      <c r="D336" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="s">
+        <v>7</v>
+      </c>
+      <c r="B337" t="s">
+        <v>1</v>
+      </c>
+      <c r="C337" t="s">
+        <v>2</v>
+      </c>
+      <c r="D337" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="s">
+        <v>7</v>
+      </c>
+      <c r="B338" t="s">
+        <v>6</v>
+      </c>
+      <c r="C338" t="s">
+        <v>4</v>
+      </c>
+      <c r="D338" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="s">
+        <v>9</v>
+      </c>
+      <c r="B339" t="s">
+        <v>1</v>
+      </c>
+      <c r="C339" t="s">
+        <v>2</v>
+      </c>
+      <c r="D339" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="s">
+        <v>9</v>
+      </c>
+      <c r="B340" t="s">
+        <v>1</v>
+      </c>
+      <c r="C340" t="s">
+        <v>4</v>
+      </c>
+      <c r="D340" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="s">
+        <v>9</v>
+      </c>
+      <c r="B341" t="s">
+        <v>6</v>
+      </c>
+      <c r="C341" t="s">
+        <v>2</v>
+      </c>
+      <c r="D341" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="s">
+        <v>9</v>
+      </c>
+      <c r="B342" t="s">
+        <v>6</v>
+      </c>
+      <c r="C342" t="s">
+        <v>4</v>
+      </c>
+      <c r="D342" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="s">
+        <v>9</v>
+      </c>
+      <c r="B343" t="s">
+        <v>1</v>
+      </c>
+      <c r="C343" t="s">
+        <v>2</v>
+      </c>
+      <c r="D343" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="s">
+        <v>9</v>
+      </c>
+      <c r="B344" t="s">
+        <v>6</v>
+      </c>
+      <c r="C344" t="s">
+        <v>4</v>
+      </c>
+      <c r="D344" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="s">
+        <v>7</v>
+      </c>
+      <c r="B345" t="s">
+        <v>1</v>
+      </c>
+      <c r="C345" t="s">
+        <v>2</v>
+      </c>
+      <c r="D345" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="s">
+        <v>7</v>
+      </c>
+      <c r="B346" t="s">
+        <v>6</v>
+      </c>
+      <c r="C346" t="s">
+        <v>4</v>
+      </c>
+      <c r="D346" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="s">
+        <v>7</v>
+      </c>
+      <c r="B347" t="s">
+        <v>1</v>
+      </c>
+      <c r="C347" t="s">
+        <v>2</v>
+      </c>
+      <c r="D347" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="s">
+        <v>19</v>
+      </c>
+      <c r="B348" t="s">
+        <v>1</v>
+      </c>
+      <c r="C348" t="s">
+        <v>2</v>
+      </c>
+      <c r="D348" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="s">
+        <v>19</v>
+      </c>
+      <c r="B349" t="s">
+        <v>1</v>
+      </c>
+      <c r="C349" t="s">
+        <v>2</v>
+      </c>
+      <c r="D349" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="s">
+        <v>19</v>
+      </c>
+      <c r="B350" t="s">
+        <v>1</v>
+      </c>
+      <c r="C350" t="s">
+        <v>2</v>
+      </c>
+      <c r="D350" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="s">
+        <v>7</v>
+      </c>
+      <c r="B351" t="s">
+        <v>1</v>
+      </c>
+      <c r="C351" t="s">
+        <v>2</v>
+      </c>
+      <c r="D351" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="s">
+        <v>9</v>
+      </c>
+      <c r="B352" t="s">
+        <v>6</v>
+      </c>
+      <c r="C352" t="s">
+        <v>2</v>
+      </c>
+      <c r="D352" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="s">
+        <v>9</v>
+      </c>
+      <c r="B353" t="s">
+        <v>1</v>
+      </c>
+      <c r="C353" t="s">
+        <v>2</v>
+      </c>
+      <c r="D353" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="s">
+        <v>9</v>
+      </c>
+      <c r="B354" t="s">
+        <v>1</v>
+      </c>
+      <c r="C354" t="s">
+        <v>2</v>
+      </c>
+      <c r="D354" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="s">
+        <v>7</v>
+      </c>
+      <c r="B355" t="s">
+        <v>6</v>
+      </c>
+      <c r="C355" t="s">
+        <v>2</v>
+      </c>
+      <c r="D355" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="s">
+        <v>9</v>
+      </c>
+      <c r="B356" t="s">
+        <v>6</v>
+      </c>
+      <c r="C356" t="s">
+        <v>2</v>
+      </c>
+      <c r="D356" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="s">
+        <v>9</v>
+      </c>
+      <c r="B357" t="s">
+        <v>6</v>
+      </c>
+      <c r="C357" t="s">
+        <v>2</v>
+      </c>
+      <c r="D357" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="s">
+        <v>9</v>
+      </c>
+      <c r="B358" t="s">
+        <v>6</v>
+      </c>
+      <c r="C358" t="s">
+        <v>2</v>
+      </c>
+      <c r="D358" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>